<commit_message>
Update IP - EX 05 - Hyperlink externo e interno (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 05 - Hyperlink externo e interno (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 05 - Hyperlink externo e interno (Anexo).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e593b6562b3551db/Dinamica_Treinamentos/Reorganização/07 - SAAS/@@EXCEL AVANÇADO/Arquivos Curso Online/Excel_Novo/Excel Intermediário/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{B1CD0BD9-9EE6-430B-927B-60574242A3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{021EE0E6-9FE9-4262-B95C-B2183B807E87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A57919C-B98E-4D51-8E60-2B08DF57C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXEMPLO" sheetId="15" r:id="rId1"/>
@@ -804,14 +804,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -830,7 +829,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
@@ -938,10 +936,10 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="7" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1171,8 +1169,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2223587" y="2352674"/>
-          <a:ext cx="1302576" cy="1080000"/>
+          <a:off x="2209507" y="2352674"/>
+          <a:ext cx="1295949" cy="1080000"/>
           <a:chOff x="4714876" y="2686049"/>
           <a:chExt cx="1296000" cy="1080000"/>
         </a:xfrm>
@@ -1333,8 +1331,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="527206" y="2352674"/>
-          <a:ext cx="1302575" cy="1080000"/>
+          <a:off x="523065" y="2352674"/>
+          <a:ext cx="1295949" cy="1080000"/>
           <a:chOff x="3028951" y="2686049"/>
           <a:chExt cx="1296000" cy="1080000"/>
         </a:xfrm>
@@ -1490,8 +1488,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2223587" y="1038224"/>
-          <a:ext cx="1302576" cy="1080000"/>
+          <a:off x="2209507" y="1038224"/>
+          <a:ext cx="1295949" cy="1080000"/>
           <a:chOff x="4714876" y="1371599"/>
           <a:chExt cx="1296000" cy="1080000"/>
         </a:xfrm>
@@ -1647,8 +1645,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="527206" y="1038224"/>
-          <a:ext cx="1302575" cy="1080000"/>
+          <a:off x="523065" y="1038224"/>
+          <a:ext cx="1295949" cy="1080000"/>
           <a:chOff x="3028951" y="1371599"/>
           <a:chExt cx="1296000" cy="1080000"/>
         </a:xfrm>
@@ -1861,8 +1859,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3361025" y="59121"/>
-          <a:ext cx="685172" cy="236482"/>
+          <a:off x="3340318" y="59121"/>
+          <a:ext cx="681859" cy="236482"/>
           <a:chOff x="3599793" y="663466"/>
           <a:chExt cx="683173" cy="236482"/>
         </a:xfrm>
@@ -2907,7 +2905,7 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="Imagem 12">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0033359-450F-45B3-B4E7-81E44839850F}"/>
@@ -2919,7 +2917,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2995,13 +2993,77 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Seta para a direita 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA0BD7E-1F80-6683-F29E-18472DDC5F48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476501" y="2571750"/>
+          <a:ext cx="533400" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 161538"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3039,9 +3101,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3074,26 +3136,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3126,26 +3171,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3321,7 +3349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E020274-661F-4E7F-BEDD-9CF89F8B2310}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3338,7 +3368,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P2"/>
+      <selection activeCell="M3" sqref="M3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,477 +3377,477 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="62"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="60"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="62"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="63" t="s">
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="62"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="60"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="62"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="60"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="62"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="60"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="63">
         <v>43819</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="27" t="s">
+      <c r="D6" s="64"/>
+      <c r="E6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="27" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="27" t="s">
+      <c r="I6" s="27"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="30"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="27" t="s">
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="62"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="60"/>
     </row>
     <row r="7" spans="1:17" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="62"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="60"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="27" t="s">
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="27" t="s">
+      <c r="I8" s="37"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="30"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="41" t="s">
+      <c r="L8" s="28"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="42"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="62"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="60"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="62"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="60"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="62"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="60"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="62"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="60"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="62"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="60"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="62"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="60"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="62"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="60"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="62"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="60"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="62"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="60"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="62"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="60"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="62"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="60"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="62"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="60"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="62"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="60"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="62"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="60"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="62"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="60"/>
     </row>
     <row r="23" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="62"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3849,8 +3879,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="B2:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3859,157 +3889,157 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="67"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="72"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="70"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="72"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="70"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="72"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="70"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="75"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="73"/>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:17" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4027,114 +4057,114 @@
   <dimension ref="B2:Q223"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="67"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="72"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="70"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="72"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="70"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="72"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="70"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="75"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="73"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="52" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4152,65 +4182,56 @@
     </row>
     <row r="15" spans="2:17" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+    <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="54" t="s">
+    <row r="19" spans="2:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="54" t="s">
+    <row r="21" spans="2:2" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
+    <row r="23" spans="2:2" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
+    <row r="25" spans="2:2" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
     </row>
     <row r="223" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C223" s="76" t="s">
+      <c r="C223" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D223" s="77"/>
-      <c r="E223" s="77"/>
-      <c r="F223" s="77"/>
-      <c r="G223" s="77"/>
-      <c r="H223" s="77"/>
-      <c r="I223" s="77"/>
-      <c r="J223" s="77"/>
-      <c r="K223" s="77"/>
-      <c r="L223" s="77"/>
-      <c r="M223" s="77"/>
-      <c r="N223" s="77"/>
-      <c r="O223" s="77"/>
-      <c r="P223" s="78"/>
+      <c r="D223" s="75"/>
+      <c r="E223" s="75"/>
+      <c r="F223" s="75"/>
+      <c r="G223" s="75"/>
+      <c r="H223" s="75"/>
+      <c r="I223" s="75"/>
+      <c r="J223" s="75"/>
+      <c r="K223" s="75"/>
+      <c r="L223" s="75"/>
+      <c r="M223" s="75"/>
+      <c r="N223" s="75"/>
+      <c r="O223" s="75"/>
+      <c r="P223" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4232,7 +4253,7 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="B2:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -4240,329 +4261,131 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="9"/>
+      <c r="B5" s="7"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="9"/>
+      <c r="B6" s="7"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="9"/>
+      <c r="B7" s="7"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="N11" s="8"/>
       <c r="P11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="9"/>
+      <c r="B12" s="7"/>
+      <c r="N12" s="8"/>
       <c r="P12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="N13" s="8"/>
       <c r="P13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="9"/>
+      <c r="B14" s="7"/>
+      <c r="N14" s="8"/>
       <c r="P14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="9"/>
+      <c r="B15" s="7"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="9"/>
+      <c r="B16" s="7"/>
+      <c r="N16" s="8"/>
       <c r="P16" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="9"/>
+      <c r="B17" s="7"/>
+      <c r="N17" s="8"/>
       <c r="P17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="9"/>
+      <c r="B18" s="7"/>
+      <c r="N18" s="8"/>
       <c r="P18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="9"/>
+      <c r="B19" s="7"/>
+      <c r="N19" s="8"/>
       <c r="P19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="9"/>
+      <c r="B20" s="7"/>
+      <c r="N20" s="8"/>
       <c r="P20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="5"/>
       <c r="P21" t="s">
         <v>8</v>

</xml_diff>